<commit_message>
Hide code and show data graphs
</commit_message>
<xml_diff>
--- a/Scripts/Data/Feedback2.xlsx
+++ b/Scripts/Data/Feedback2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentdkit-my.sharepoint.com/personal/d00248313_student_dkit_ie/Documents/Documents/HolyDead_Surveys_Analysis/Scripts/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF92B555-B161-4F3B-9C17-56FB17032017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{FF92B555-B161-4F3B-9C17-56FB17032017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D092C822-B2BC-4E28-AC08-7321DB3F8480}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7380" yWindow="1476" windowWidth="15660" windowHeight="10764" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -478,7 +478,7 @@
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
     <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{839C7E11-91E4-4DBD-9C5D-0DEA604FA9AC}">
-      <xlmsforms:msForm id="S5rMqwTPo0ydgzRl4_Q_YS7B5bmCEedGqxVOMgN6-VRUQ1U4T081N1VSOFRDSlBHRDRUOFQyWDk4TC4u" isFormConnected="1" maxResponseId="16" latestEventMarker="0">
+      <xlmsforms:msForm id="S5rMqwTPo0ydgzRl4_Q_YS7B5bmCEedGqxVOMgN6-VRUQ1U4T081N1VSOFRDSlBHRDRUOFQyWDk4TC4u" maxResponseId="16" latestEventMarker="0">
         <xlmsforms:syncedQuestionId>id</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>startDate</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>submitDate</xlmsforms:syncedQuestionId>

</xml_diff>